<commit_message>
Modified DSL for Tabbar, notification and adding new screenshots
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Application_Ruby.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Application_Ruby.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -438,12 +438,6 @@
 {
 validate_Result=/data/data/com.rhomobile.compliancetestruby/rhodata/db/syncdblocal.sqlite
 };</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <t>set Native menu to different actions</t>
@@ -1001,9 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1057,9 +1049,11 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="4" t="s">
         <v>68</v>
       </c>
@@ -1075,9 +1069,7 @@
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="230.25" thickBot="1">
@@ -1088,7 +1080,9 @@
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1102,9 +1096,7 @@
         <v>77</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="243" thickBot="1">
@@ -1115,7 +1107,9 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
@@ -1129,9 +1123,7 @@
         <v>81</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="230.25" thickBot="1">
@@ -1142,7 +1134,9 @@
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>29</v>
       </c>
@@ -1156,9 +1150,7 @@
         <v>78</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="230.25" thickBot="1">
@@ -1169,7 +1161,9 @@
         <v>1</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>71</v>
       </c>
@@ -1183,9 +1177,7 @@
         <v>79</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="230.25" thickBot="1">
@@ -1196,7 +1188,9 @@
         <v>1</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E7" s="13" t="s">
         <v>51</v>
       </c>
@@ -1210,9 +1204,7 @@
         <v>80</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="179.25" thickBot="1">
@@ -1223,23 +1215,23 @@
         <v>1</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>86</v>
-      </c>
       <c r="H8" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>82</v>
-      </c>
+      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="281.25" thickBot="1">
@@ -1254,21 +1246,19 @@
         <v>10</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>89</v>
-      </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
   </sheetData>

</xml_diff>